<commit_message>
Nå er budsjettet oppdatert
</commit_message>
<xml_diff>
--- a/regneark.xlsx
+++ b/regneark.xlsx
@@ -1,33 +1,77 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jokane\Dropbox\JornGit2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AAE355-4DBA-40C8-B11F-ED745E4ECCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0123A5A3-4717-4F27-A833-27BDB3823096}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="420" windowWidth="14400" windowHeight="8904" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Budsjett</t>
+  </si>
+  <si>
+    <t>inntekter</t>
+  </si>
+  <si>
+    <t>lønn</t>
+  </si>
+  <si>
+    <t>salg av div</t>
+  </si>
+  <si>
+    <t>Inntekt totalt</t>
+  </si>
+  <si>
+    <t>Utgifter</t>
+  </si>
+  <si>
+    <t>Husleie</t>
+  </si>
+  <si>
+    <t>Drivstoff</t>
+  </si>
+  <si>
+    <t>Mat</t>
+  </si>
+  <si>
+    <t>Strøm</t>
+  </si>
+  <si>
+    <t>Forsikringer</t>
+  </si>
+  <si>
+    <t>Abonnementer</t>
   </si>
 </sst>
 </file>
@@ -345,17 +389,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f>SUM(B3:B4)</f>
+        <v>7300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>